<commit_message>
updated models, results to sep-15
</commit_message>
<xml_diff>
--- a/models/Sentence_based/stage_1_matrix_forecast.xlsx
+++ b/models/Sentence_based/stage_1_matrix_forecast.xlsx
@@ -390,10 +390,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>49150</v>
+        <v>64657</v>
       </c>
       <c r="C3" t="n">
-        <v>105776</v>
+        <v>120513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>